<commit_message>
9 hours coding session: END
</commit_message>
<xml_diff>
--- a/Labb2/betyg_o_prov_riksnivå.xlsx
+++ b/Labb2/betyg_o_prov_riksnivå.xlsx
@@ -3458,12 +3458,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="17" width="3.1478571428571427" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="17" width="48.86214285714286" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="17" width="9.147857142857141" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="17" width="9.147857142857141" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="17" width="9.147857142857141" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="17" width="8.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="17" width="9.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="17" width="95.86214285714286" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="17" width="9.147857142857141" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="17" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="9" max="9" style="17" width="14.147857142857141" customWidth="1" bestFit="1"/>

</xml_diff>